<commit_message>
cont mode might be fixed
</commit_message>
<xml_diff>
--- a/간트차트 (자동 저장됨).xlsx
+++ b/간트차트 (자동 저장됨).xlsx
@@ -203,11 +203,11 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>7. Multi thread issue. Critical section setting으로 보여짐</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>8. Camera Open / Close도 Thread 요망</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Thread 갈아엎기..</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -2102,7 +2102,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2200,7 +2200,7 @@
         <v>11.09</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2210,7 +2210,7 @@
         <v>11.09</v>
       </c>
       <c r="D8" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4">

</xml_diff>

<commit_message>
this is currently done project.. image view has no problem but wants some class repositioning and bug fixes.
</commit_message>
<xml_diff>
--- a/간트차트 (자동 저장됨).xlsx
+++ b/간트차트 (자동 저장됨).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>11 월</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -216,6 +216,14 @@
   </si>
   <si>
     <t>9. 이미지 뷰어는 현재 SW Trigger 일 때만 동작 (DrawImageSeq에서 SW Trigger 파트에서만)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>issue1</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -409,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -857,6 +865,78 @@
     <border>
       <left/>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -882,7 +962,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -955,9 +1035,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1003,6 +1080,36 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1420,73 +1527,73 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="17.25" thickBot="1">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="59"/>
-      <c r="V5" s="59"/>
-      <c r="W5" s="59"/>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="60"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="59"/>
     </row>
     <row r="6" spans="1:25" ht="17.25" thickBot="1">
-      <c r="B6" s="56"/>
-      <c r="C6" s="58" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="60"/>
-      <c r="E6" s="58" t="s">
+      <c r="D6" s="59"/>
+      <c r="E6" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="58" t="s">
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="58" t="s">
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="60"/>
-      <c r="T6" s="58" t="s">
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="59"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="60"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="58"/>
+      <c r="Y6" s="59"/>
     </row>
     <row r="7" spans="1:25" ht="17.25" thickBot="1">
-      <c r="B7" s="57"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="26">
         <v>44133</v>
       </c>
@@ -2107,222 +2214,253 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="53"/>
-    <col min="2" max="2" width="69.625" style="43" customWidth="1"/>
-    <col min="3" max="3" width="9" style="53"/>
-    <col min="4" max="4" width="87.625" style="43" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="43"/>
+    <col min="1" max="1" width="9" style="52"/>
+    <col min="2" max="2" width="69.625" style="42" customWidth="1"/>
+    <col min="3" max="4" width="9" style="52"/>
+    <col min="5" max="5" width="87.625" style="42" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" thickBot="1">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:5" ht="17.25" thickBot="1">
+      <c r="A1" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="36">
         <v>11.02</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="61">
         <v>11.02</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="44" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="37">
         <v>11.02</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="62">
         <v>11.05</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="65"/>
+      <c r="E3" s="46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="37">
         <v>11.03</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="62">
         <v>11.05</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="65"/>
+      <c r="E4" s="46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="37">
         <v>11.05</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="62">
         <v>11.06</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="65"/>
+      <c r="E5" s="46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="37"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="38">
+      <c r="B6" s="47"/>
+      <c r="C6" s="63">
         <v>11.06</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="65"/>
+      <c r="E6" s="46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="37"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="54"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" s="47"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="53"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="37"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="36">
+      <c r="B8" s="47"/>
+      <c r="C8" s="61">
         <v>11.09</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="48" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="37"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="37" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="68"/>
+      <c r="E9" s="48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="37"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="37" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="69"/>
+      <c r="E10" s="48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="37"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="50"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11" s="47"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="49"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="37"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="50"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" s="47"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="49"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="37"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="50"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="B13" s="47"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="49"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="37"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="50"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="B14" s="47"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="49"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="37"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="50"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="B15" s="47"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="49"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="37"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="50"/>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="B16" s="47"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="49"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="37"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="50"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" s="47"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="49"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="37"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="50"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="B18" s="47"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="49"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="37"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="50"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="B19" s="47"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="49"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="37"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="50"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="B20" s="47"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="49"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="37"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="50"/>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="B21" s="47"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="49"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="37"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="50"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="B22" s="47"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="49"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="37"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="50"/>
-    </row>
-    <row r="24" spans="1:4" ht="17.25" thickBot="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="52"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="49"/>
+    </row>
+    <row r="24" spans="1:5" ht="17.25" thickBot="1">
+      <c r="A24" s="38"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="51"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D8:D10"/>
+  </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
opencv test done... it works | light test btn bug fixed
</commit_message>
<xml_diff>
--- a/간트차트 (자동 저장됨).xlsx
+++ b/간트차트 (자동 저장됨).xlsx
@@ -1229,7 +1229,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="5" applyAlignment="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1260,6 +1259,7 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - 강조색1" xfId="6" builtinId="30"/>
@@ -1749,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1775,73 +1775,73 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="71"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="69"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="69"/>
+      <c r="Y5" s="70"/>
     </row>
     <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="67"/>
-      <c r="C6" s="69" t="s">
+      <c r="B6" s="66"/>
+      <c r="C6" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="69" t="s">
+      <c r="D6" s="70"/>
+      <c r="E6" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="69" t="s">
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="69" t="s">
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="69" t="s">
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="U6" s="70"/>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70"/>
-      <c r="X6" s="70"/>
-      <c r="Y6" s="71"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="69"/>
+      <c r="X6" s="69"/>
+      <c r="Y6" s="70"/>
     </row>
     <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="68"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="24">
         <v>44133</v>
       </c>
@@ -2373,8 +2373,8 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="26"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="1"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -2429,7 +2429,7 @@
       <c r="J26" s="59"/>
       <c r="K26" s="59"/>
       <c r="L26" s="59"/>
-      <c r="M26" s="64"/>
+      <c r="M26" s="74"/>
       <c r="N26" s="59"/>
       <c r="O26" s="59"/>
       <c r="P26" s="59"/>
@@ -2606,7 +2606,7 @@
       <c r="C8" s="50">
         <v>11.09</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="71" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="42" t="s">
@@ -2619,7 +2619,7 @@
       <c r="C9" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="73"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="42" t="s">
         <v>15</v>
       </c>
@@ -2630,7 +2630,7 @@
       <c r="C10" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="44" t="s">
         <v>16</v>
       </c>
@@ -2641,7 +2641,7 @@
       <c r="C11" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="74"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="44" t="s">
         <v>19</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="A24" s="34"/>
       <c r="B24" s="46"/>
       <c r="C24" s="53"/>
-      <c r="D24" s="65"/>
+      <c r="D24" s="64"/>
       <c r="E24" s="47"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gray level done | picture control db click set done
</commit_message>
<xml_diff>
--- a/간트차트 (자동 저장됨).xlsx
+++ b/간트차트 (자동 저장됨).xlsx
@@ -1232,6 +1232,7 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1259,7 +1260,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - 강조색1" xfId="6" builtinId="30"/>
@@ -1750,7 +1750,7 @@
   <dimension ref="A2:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1775,73 +1775,73 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69"/>
-      <c r="W5" s="69"/>
-      <c r="X5" s="69"/>
-      <c r="Y5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="71"/>
     </row>
     <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="66"/>
-      <c r="C6" s="68" t="s">
+      <c r="B6" s="67"/>
+      <c r="C6" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="68" t="s">
+      <c r="D6" s="71"/>
+      <c r="E6" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="68" t="s">
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="68" t="s">
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="68" t="s">
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="U6" s="69"/>
-      <c r="V6" s="69"/>
-      <c r="W6" s="69"/>
-      <c r="X6" s="69"/>
-      <c r="Y6" s="70"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="70"/>
+      <c r="W6" s="70"/>
+      <c r="X6" s="70"/>
+      <c r="Y6" s="71"/>
     </row>
     <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="67"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="24">
         <v>44133</v>
       </c>
@@ -2290,10 +2290,10 @@
       <c r="K21" s="1"/>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -2429,7 +2429,7 @@
       <c r="J26" s="59"/>
       <c r="K26" s="59"/>
       <c r="L26" s="59"/>
-      <c r="M26" s="74"/>
+      <c r="M26" s="65"/>
       <c r="N26" s="59"/>
       <c r="O26" s="59"/>
       <c r="P26" s="59"/>
@@ -2606,7 +2606,7 @@
       <c r="C8" s="50">
         <v>11.09</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="72" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="42" t="s">
@@ -2619,7 +2619,7 @@
       <c r="C9" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="72"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="42" t="s">
         <v>15</v>
       </c>
@@ -2630,7 +2630,7 @@
       <c r="C10" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="72"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="44" t="s">
         <v>16</v>
       </c>
@@ -2641,7 +2641,7 @@
       <c r="C11" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="73"/>
+      <c r="D11" s="74"/>
       <c r="E11" s="44" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
magnifier made ! ! have to set grid but 귀찮아
</commit_message>
<xml_diff>
--- a/간트차트 (자동 저장됨).xlsx
+++ b/간트차트 (자동 저장됨).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="간트" sheetId="1" r:id="rId1"/>
@@ -1749,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2093,7 +2093,7 @@
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
-      <c r="M14" s="21"/>
+      <c r="M14" s="31"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -2372,9 +2372,9 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -2492,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2642,7 +2642,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="74"/>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="42" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
larger screen ongoing, bug exists (rgb value get bug)
</commit_message>
<xml_diff>
--- a/간트차트 (자동 저장됨).xlsx
+++ b/간트차트 (자동 저장됨).xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>1. Open 버튼 구현 시 option.ini 파일을 읽어야 할 것 같음</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -331,6 +331,14 @@
     <t>- 중간 점검 및 Issue fix</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>11.16</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>x,y 이동 방향 파악하는 법 강구하기</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -339,7 +347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm\.dd"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1104,7 +1112,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1260,6 +1268,7 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - 강조색1" xfId="6" builtinId="30"/>
@@ -1753,28 +1762,28 @@
       <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="40.625" customWidth="1"/>
     <col min="3" max="25" width="6.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" ht="17.25" thickBot="1">
       <c r="A4" s="27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="17.25" thickBot="1">
       <c r="B5" s="66" t="s">
         <v>24</v>
       </c>
@@ -1804,7 +1813,7 @@
       <c r="X5" s="70"/>
       <c r="Y5" s="71"/>
     </row>
-    <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="17.25" thickBot="1">
       <c r="B6" s="67"/>
       <c r="C6" s="69" t="s">
         <v>26</v>
@@ -1840,7 +1849,7 @@
       <c r="X6" s="70"/>
       <c r="Y6" s="71"/>
     </row>
-    <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="17.25" thickBot="1">
       <c r="B7" s="68"/>
       <c r="C7" s="24">
         <v>44133</v>
@@ -1912,7 +1921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="17.25" thickBot="1">
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1940,7 +1949,7 @@
       <c r="X8" s="12"/>
       <c r="Y8" s="13"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="B9" s="56" t="s">
         <v>32</v>
       </c>
@@ -1967,7 +1976,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="B10" s="56" t="s">
         <v>33</v>
       </c>
@@ -1995,7 +2004,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="B11" s="8" t="s">
         <v>34</v>
       </c>
@@ -2023,7 +2032,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="B12" s="8" t="s">
         <v>35</v>
       </c>
@@ -2051,7 +2060,7 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="B13" s="8" t="s">
         <v>36</v>
       </c>
@@ -2079,7 +2088,7 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="17.25" thickBot="1">
       <c r="B14" s="9" t="s">
         <v>37</v>
       </c>
@@ -2107,7 +2116,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="17.25" thickBot="1">
       <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
@@ -2135,7 +2144,7 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="B16" s="7" t="s">
         <v>39</v>
       </c>
@@ -2163,7 +2172,7 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:25">
       <c r="B17" s="8" t="s">
         <v>40</v>
       </c>
@@ -2191,7 +2200,7 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:25">
       <c r="B18" s="19" t="s">
         <v>41</v>
       </c>
@@ -2219,7 +2228,7 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:25" ht="17.25" thickBot="1">
       <c r="B19" s="57" t="s">
         <v>42</v>
       </c>
@@ -2247,7 +2256,7 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:25" ht="17.25" thickBot="1">
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
@@ -2275,7 +2284,7 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:25">
       <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
@@ -2303,7 +2312,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:25">
       <c r="B22" s="8" t="s">
         <v>45</v>
       </c>
@@ -2331,7 +2340,7 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:25">
       <c r="B23" s="8" t="s">
         <v>46</v>
       </c>
@@ -2359,7 +2368,7 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:25" ht="17.25" thickBot="1">
       <c r="B24" s="9" t="s">
         <v>47</v>
       </c>
@@ -2387,7 +2396,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:25" ht="17.25" thickBot="1">
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
@@ -2415,7 +2424,7 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:25">
       <c r="B26" s="61" t="s">
         <v>50</v>
       </c>
@@ -2443,7 +2452,7 @@
       <c r="X26" s="59"/>
       <c r="Y26" s="60"/>
     </row>
-    <row r="27" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:25" ht="17.25" thickBot="1">
       <c r="B27" s="10" t="s">
         <v>49</v>
       </c>
@@ -2490,13 +2499,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9" style="48"/>
     <col min="2" max="2" width="69.625" style="38" customWidth="1"/>
@@ -2505,7 +2514,7 @@
     <col min="6" max="16384" width="9" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="17.25" thickBot="1">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -2522,7 +2531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="32">
         <v>11.02</v>
       </c>
@@ -2537,7 +2546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="33">
         <v>11.02</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="33">
         <v>11.03</v>
       </c>
@@ -2567,7 +2576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="33">
         <v>11.05</v>
       </c>
@@ -2582,7 +2591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="33"/>
       <c r="B6" s="43"/>
       <c r="C6" s="52">
@@ -2593,14 +2602,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="33"/>
       <c r="B7" s="43"/>
       <c r="C7" s="51"/>
       <c r="D7" s="54"/>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="75"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="33"/>
       <c r="B8" s="43"/>
       <c r="C8" s="50">
@@ -2613,7 +2623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="33"/>
       <c r="B9" s="43"/>
       <c r="C9" s="51" t="s">
@@ -2624,7 +2634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="33"/>
       <c r="B10" s="43"/>
       <c r="C10" s="51" t="s">
@@ -2635,7 +2645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="33"/>
       <c r="B11" s="43"/>
       <c r="C11" s="51" t="s">
@@ -2646,91 +2656,95 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="33"/>
       <c r="B12" s="43"/>
-      <c r="C12" s="51"/>
+      <c r="C12" s="51" t="s">
+        <v>51</v>
+      </c>
       <c r="D12" s="54"/>
-      <c r="E12" s="45"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="33"/>
       <c r="B13" s="43"/>
       <c r="C13" s="51"/>
       <c r="D13" s="54"/>
       <c r="E13" s="45"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="33"/>
       <c r="B14" s="43"/>
       <c r="C14" s="51"/>
       <c r="D14" s="54"/>
       <c r="E14" s="45"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="33"/>
       <c r="B15" s="43"/>
       <c r="C15" s="51"/>
       <c r="D15" s="54"/>
       <c r="E15" s="45"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16" s="33"/>
       <c r="B16" s="43"/>
       <c r="C16" s="51"/>
       <c r="D16" s="54"/>
       <c r="E16" s="45"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="33"/>
       <c r="B17" s="43"/>
       <c r="C17" s="51"/>
       <c r="D17" s="54"/>
       <c r="E17" s="45"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="33"/>
       <c r="B18" s="43"/>
       <c r="C18" s="51"/>
       <c r="D18" s="54"/>
       <c r="E18" s="45"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="33"/>
       <c r="B19" s="43"/>
       <c r="C19" s="51"/>
       <c r="D19" s="54"/>
       <c r="E19" s="45"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="33"/>
       <c r="B20" s="43"/>
       <c r="C20" s="51"/>
       <c r="D20" s="54"/>
       <c r="E20" s="45"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="33"/>
       <c r="B21" s="43"/>
       <c r="C21" s="51"/>
       <c r="D21" s="54"/>
       <c r="E21" s="45"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="33"/>
       <c r="B22" s="43"/>
       <c r="C22" s="51"/>
       <c r="D22" s="54"/>
       <c r="E22" s="45"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" s="33"/>
       <c r="B23" s="43"/>
       <c r="C23" s="51"/>
       <c r="D23" s="54"/>
       <c r="E23" s="45"/>
     </row>
-    <row r="24" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="17.25" thickBot="1">
       <c r="A24" s="34"/>
       <c r="B24" s="46"/>
       <c r="C24" s="53"/>

</xml_diff>

<commit_message>
cursor ROI, thresh done
</commit_message>
<xml_diff>
--- a/간트차트 (자동 저장됨).xlsx
+++ b/간트차트 (자동 저장됨).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="간트" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>1. Open 버튼 구현 시 option.ini 파일을 읽어야 할 것 같음</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -336,7 +336,15 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>x,y 이동 방향 파악하는 법 강구하기</t>
+    <t>11.17</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>x,y 이동 방향 파악하는 법 강구하기 (약간 이상함)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>y축으로 맨 밑에 확대 Rect가 닿을때 이상함..</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -347,7 +355,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm\.dd"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1134,7 +1142,6 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="16" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1241,6 +1248,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1268,7 +1276,7 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - 강조색1" xfId="6" builtinId="30"/>
@@ -1758,32 +1766,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="40.625" customWidth="1"/>
     <col min="3" max="25" width="6.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="17.25" thickBot="1">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="17.25" thickBot="1">
+    <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="66" t="s">
         <v>24</v>
       </c>
@@ -1813,7 +1821,7 @@
       <c r="X5" s="70"/>
       <c r="Y5" s="71"/>
     </row>
-    <row r="6" spans="1:25" ht="17.25" thickBot="1">
+    <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="67"/>
       <c r="C6" s="69" t="s">
         <v>26</v>
@@ -1849,120 +1857,120 @@
       <c r="X6" s="70"/>
       <c r="Y6" s="71"/>
     </row>
-    <row r="7" spans="1:25" ht="17.25" thickBot="1">
+    <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="68"/>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>44133</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <v>44134</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>2</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>3</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="16">
         <v>4</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="16">
         <v>5</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="16">
         <v>6</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="16">
         <v>9</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="16">
         <v>10</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="16">
         <v>11</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="16">
         <v>12</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="16">
         <v>13</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="16">
         <v>16</v>
       </c>
-      <c r="P7" s="17">
+      <c r="P7" s="16">
         <v>17</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="16">
         <v>18</v>
       </c>
-      <c r="R7" s="17">
+      <c r="R7" s="16">
         <v>19</v>
       </c>
-      <c r="S7" s="17">
+      <c r="S7" s="16">
         <v>20</v>
       </c>
-      <c r="T7" s="17">
+      <c r="T7" s="16">
         <v>23</v>
       </c>
-      <c r="U7" s="17">
+      <c r="U7" s="16">
         <v>24</v>
       </c>
-      <c r="V7" s="17">
+      <c r="V7" s="16">
         <v>25</v>
       </c>
-      <c r="W7" s="17">
+      <c r="W7" s="16">
         <v>26</v>
       </c>
-      <c r="X7" s="17">
+      <c r="X7" s="16">
         <v>27</v>
       </c>
-      <c r="Y7" s="18">
+      <c r="Y7" s="17">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="17.25" thickBot="1">
+    <row r="8" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="13"/>
-    </row>
-    <row r="9" spans="1:25">
-      <c r="B9" s="56" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="12"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B9" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="F9" s="23"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="21"/>
+      <c r="M9" s="20"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1976,21 +1984,21 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:25">
-      <c r="B10" s="56" t="s">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B10" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="21"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -2004,21 +2012,21 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="21"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -2032,21 +2040,21 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="21"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -2060,21 +2068,21 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="23"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="22"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="21"/>
+      <c r="M13" s="20"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -2088,21 +2096,21 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" ht="17.25" thickBot="1">
+    <row r="14" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -2116,7 +2124,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" ht="17.25" thickBot="1">
+    <row r="15" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
@@ -2130,7 +2138,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="21"/>
+      <c r="M15" s="20"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -2144,7 +2152,7 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>39</v>
       </c>
@@ -2153,12 +2161,12 @@
       <c r="E16" s="4"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="21"/>
+      <c r="M16" s="20"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -2172,7 +2180,7 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="2:25">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
         <v>40</v>
       </c>
@@ -2181,12 +2189,12 @@
       <c r="E17" s="4"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="21"/>
+      <c r="M17" s="20"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -2200,21 +2208,21 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="2:25">
-      <c r="B18" s="19" t="s">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="21"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -2228,8 +2236,8 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="2:25" ht="17.25" thickBot="1">
-      <c r="B19" s="57" t="s">
+    <row r="19" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="56" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="4"/>
@@ -2239,10 +2247,10 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -2256,7 +2264,7 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="2:25" ht="17.25" thickBot="1">
+    <row r="20" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
@@ -2270,7 +2278,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="21"/>
+      <c r="M20" s="20"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -2284,7 +2292,7 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="2:25">
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
@@ -2297,12 +2305,11 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -2312,7 +2319,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="2:25">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
         <v>45</v>
       </c>
@@ -2326,21 +2333,21 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="21"/>
+      <c r="M22" s="20"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="25"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="2:25">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>46</v>
       </c>
@@ -2354,7 +2361,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="21"/>
+      <c r="M23" s="20"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2362,13 +2369,13 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="2:25" ht="17.25" thickBot="1">
+    <row r="24" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="9" t="s">
         <v>47</v>
       </c>
@@ -2381,9 +2388,9 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -2396,7 +2403,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="2:25" ht="17.25" thickBot="1">
+    <row r="25" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
@@ -2410,7 +2417,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="21"/>
+      <c r="M25" s="20"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -2424,35 +2431,35 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="2:25">
-      <c r="B26" s="61" t="s">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B26" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59"/>
-      <c r="T26" s="59"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="59"/>
-      <c r="W26" s="59"/>
-      <c r="X26" s="59"/>
-      <c r="Y26" s="60"/>
-    </row>
-    <row r="27" spans="2:25" ht="17.25" thickBot="1">
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="58"/>
+      <c r="Y26" s="59"/>
+    </row>
+    <row r="27" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10" t="s">
         <v>49</v>
       </c>
@@ -2466,7 +2473,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="63"/>
+      <c r="M27" s="62"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -2477,8 +2484,8 @@
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
-      <c r="X27" s="3"/>
-      <c r="Y27" s="15"/>
+      <c r="X27" s="75"/>
+      <c r="Y27" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2501,255 +2508,259 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="48"/>
-    <col min="2" max="2" width="69.625" style="38" customWidth="1"/>
-    <col min="3" max="4" width="9" style="48"/>
-    <col min="5" max="5" width="87.625" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="38"/>
+    <col min="1" max="1" width="9" style="47"/>
+    <col min="2" max="2" width="69.625" style="37" customWidth="1"/>
+    <col min="3" max="4" width="9" style="47"/>
+    <col min="5" max="5" width="87.625" style="37" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="32">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="31">
         <v>11.02</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50">
+      <c r="C2" s="49">
         <v>11.02</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="40" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="33">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="32">
         <v>11.02</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="50">
         <v>11.05</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="42" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="33">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="32">
         <v>11.03</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="50">
         <v>11.05</v>
       </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="42" t="s">
+      <c r="D4" s="53"/>
+      <c r="E4" s="41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="33">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="32">
         <v>11.05</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="50">
         <v>11.06</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="42" t="s">
+      <c r="D5" s="53"/>
+      <c r="E5" s="41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="33"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="52">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="32"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="51">
         <v>11.06</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="42" t="s">
+      <c r="D6" s="53"/>
+      <c r="E6" s="41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="33"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="54"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="32"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="75"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="33"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="50">
+      <c r="F7" s="65"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="32"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="49">
         <v>11.09</v>
       </c>
       <c r="D8" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="33"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="51" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="32"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="73"/>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="33"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="51" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="50" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="73"/>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="43" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="33"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="51" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="32"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="50" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="74"/>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="41" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="33"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="51" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="32"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="45" t="s">
+      <c r="D12" s="53"/>
+      <c r="E12" s="43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="50" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="33"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="45"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="33"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="45"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="33"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="45"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="33"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="45"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="33"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="45"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="33"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="45"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="33"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="45"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="33"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="45"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="33"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="45"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="33"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="45"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="33"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="45"/>
-    </row>
-    <row r="24" spans="1:5" ht="17.25" thickBot="1">
-      <c r="A24" s="34"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="47"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="44"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="44"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="44"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="32"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="44"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="32"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="44"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="44"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="32"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="44"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="44"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="44"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="44"/>
+    </row>
+    <row r="24" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="33"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
image viewer complete : glitchy part removed for now
</commit_message>
<xml_diff>
--- a/간트차트 (자동 저장됨).xlsx
+++ b/간트차트 (자동 저장됨).xlsx
@@ -108,12 +108,134 @@
         </r>
       </text>
     </comment>
+    <comment ref="E13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>만든 이:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">
+근본적</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>원인</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> : rgbv get</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">때
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>height</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>값이</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이상하게</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>잡힘</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>1. Open 버튼 구현 시 option.ini 파일을 읽어야 할 것 같음</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -340,11 +462,35 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>x,y 이동 방향 파악하는 법 강구하기 (약간 이상함)</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>y축으로 맨 밑에 확대 Rect가 닿을때 이상함..</t>
+    <t>11.18</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.18</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>11. x,y 이동 방향 파악하는 법 강구하기 (약간 이상함)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>13. cursor 확대 x축 화면 맨 오른쪽 닿을때 AccessViolation</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>14. cursor 확대 y축 화면 맨 하단 닿을때 AccessViolation</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.19</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>15. 확대 후 drag시 cursor 확대 화면 좌표 밀림현상</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>12 .y축으로 맨 밑에 확대 Rect가 닿을때 AccessViolation</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -355,7 +501,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm\.dd"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,8 +641,24 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,6 +703,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="43">
     <border>
@@ -1099,7 +1266,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -1119,8 +1286,11 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1145,7 +1315,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1249,6 +1418,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1276,11 +1446,14 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="18" fillId="9" borderId="31" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="20% - 강조색1" xfId="6" builtinId="30"/>
     <cellStyle name="20% - 강조색5" xfId="4" builtinId="46"/>
+    <cellStyle name="나쁨" xfId="7" builtinId="27"/>
     <cellStyle name="메모" xfId="2" builtinId="10"/>
     <cellStyle name="보통" xfId="5" builtinId="28"/>
     <cellStyle name="입력" xfId="3" builtinId="20"/>
@@ -1777,17 +1950,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1859,73 +2032,73 @@
     </row>
     <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="68"/>
-      <c r="C7" s="23">
+      <c r="C7" s="22">
         <v>44133</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>44134</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>2</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="15">
         <v>3</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>4</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <v>5</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="15">
         <v>6</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="15">
         <v>9</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="15">
         <v>10</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="15">
         <v>11</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="15">
         <v>12</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="15">
         <v>13</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="15">
         <v>16</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="15">
         <v>17</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="15">
         <v>18</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="15">
         <v>19</v>
       </c>
-      <c r="S7" s="16">
+      <c r="S7" s="15">
         <v>20</v>
       </c>
-      <c r="T7" s="16">
+      <c r="T7" s="15">
         <v>23</v>
       </c>
-      <c r="U7" s="16">
+      <c r="U7" s="15">
         <v>24</v>
       </c>
-      <c r="V7" s="16">
+      <c r="V7" s="15">
         <v>25</v>
       </c>
-      <c r="W7" s="16">
+      <c r="W7" s="15">
         <v>26</v>
       </c>
-      <c r="X7" s="16">
+      <c r="X7" s="15">
         <v>27</v>
       </c>
-      <c r="Y7" s="17">
+      <c r="Y7" s="16">
         <v>30</v>
       </c>
     </row>
@@ -1943,7 +2116,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
-      <c r="M8" s="61"/>
+      <c r="M8" s="60"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
@@ -1958,19 +2131,19 @@
       <c r="Y8" s="12"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="F9" s="22"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="20"/>
+      <c r="M9" s="19"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1985,20 +2158,20 @@
       <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="20"/>
+      <c r="M10" s="19"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -2016,17 +2189,17 @@
       <c r="B11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="20"/>
+      <c r="M11" s="19"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -2044,17 +2217,17 @@
       <c r="B12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="20"/>
+      <c r="M12" s="19"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -2075,14 +2248,14 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="22"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="20"/>
+      <c r="M13" s="19"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -2103,14 +2276,14 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -2138,7 +2311,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="20"/>
+      <c r="M15" s="19"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -2161,12 +2334,12 @@
       <c r="E16" s="4"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="20"/>
+      <c r="M16" s="19"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -2189,12 +2362,12 @@
       <c r="E17" s="4"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="20"/>
+      <c r="M17" s="19"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -2209,20 +2382,20 @@
       <c r="Y17" s="2"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="19"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="20"/>
+      <c r="M18" s="19"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -2237,7 +2410,7 @@
       <c r="Y18" s="2"/>
     </row>
     <row r="19" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="55" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="4"/>
@@ -2247,10 +2420,10 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -2278,7 +2451,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="20"/>
+      <c r="M20" s="19"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -2305,11 +2478,11 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
@@ -2333,17 +2506,17 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="20"/>
+      <c r="M22" s="19"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="25"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="2"/>
     </row>
@@ -2361,17 +2534,17 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="20"/>
+      <c r="M23" s="19"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="25"/>
-      <c r="V23" s="25"/>
-      <c r="W23" s="25"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="2"/>
     </row>
@@ -2388,9 +2561,9 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -2417,7 +2590,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="20"/>
+      <c r="M25" s="19"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -2432,32 +2605,32 @@
       <c r="Y25" s="2"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="58"/>
-      <c r="S26" s="58"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="58"/>
-      <c r="V26" s="58"/>
-      <c r="W26" s="58"/>
-      <c r="X26" s="58"/>
-      <c r="Y26" s="59"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="57"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="58"/>
     </row>
     <row r="27" spans="2:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10" t="s">
@@ -2473,7 +2646,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="62"/>
+      <c r="M27" s="61"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -2483,9 +2656,9 @@
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
+      <c r="W27" s="65"/>
       <c r="X27" s="75"/>
-      <c r="Y27" s="14"/>
+      <c r="Y27" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2508,259 +2681,271 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="47"/>
-    <col min="2" max="2" width="69.625" style="37" customWidth="1"/>
-    <col min="3" max="4" width="9" style="47"/>
-    <col min="5" max="5" width="87.625" style="37" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="37"/>
+    <col min="1" max="1" width="9" style="46"/>
+    <col min="2" max="2" width="69.625" style="36" customWidth="1"/>
+    <col min="3" max="4" width="9" style="46"/>
+    <col min="5" max="5" width="87.625" style="36" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="31">
+      <c r="A2" s="30">
         <v>11.02</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="48">
         <v>11.02</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="39" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="38" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="32">
+      <c r="A3" s="31">
         <v>11.02</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="50">
+      <c r="C3" s="49">
         <v>11.05</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="41" t="s">
+      <c r="D3" s="52"/>
+      <c r="E3" s="40" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="32">
+      <c r="A4" s="31">
         <v>11.03</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="50">
+      <c r="C4" s="49">
         <v>11.05</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="41" t="s">
+      <c r="D4" s="52"/>
+      <c r="E4" s="40" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="32">
+      <c r="A5" s="31">
         <v>11.05</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="49">
         <v>11.06</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="41" t="s">
+      <c r="D5" s="52"/>
+      <c r="E5" s="40" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="51">
+      <c r="A6" s="31"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="50">
         <v>11.06</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="41" t="s">
+      <c r="D6" s="52"/>
+      <c r="E6" s="40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="53"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="65"/>
+      <c r="F7" s="64"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="49">
+      <c r="A8" s="31"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="48">
         <v>11.09</v>
       </c>
       <c r="D8" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="40" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="50" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="73"/>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="40" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="50" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="49" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="73"/>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="42" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="50" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="49" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="74"/>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="40" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="50" t="s">
+      <c r="A12" s="31"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="43" t="s">
+      <c r="D12" s="52"/>
+      <c r="E12" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="31"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="52"/>
+      <c r="E13" s="42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="31"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="49" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="44" t="s">
+      <c r="D14" s="52"/>
+      <c r="E14" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="31"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="49" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="44"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="44"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="42" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="44"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="52"/>
+      <c r="E16" s="77" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="44"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="43"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="44"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="43"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="44"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="43"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="44"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="43"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="44"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="43"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="44"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="43"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="44"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="43"/>
     </row>
     <row r="24" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="33"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="46"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>